<commit_message>
Documento Requisitos (Excel) atualizado
</commit_message>
<xml_diff>
--- a/DocRequisitos.xlsx
+++ b/DocRequisitos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Joao\UMINHO\UC\BD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5071B6D2-C719-4B2C-88A4-69C1B748B860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E4D54C1-873D-4C59-8FE7-C99B05A36E17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="51">
   <si>
     <t>Processo de Desenvolvimento do Sistema de Bases de Dados</t>
   </si>
@@ -123,12 +123,6 @@
     <t>A competição possuí diversos funcionários</t>
   </si>
   <si>
-    <t>R05</t>
-  </si>
-  <si>
-    <t>Cada funcionário tem um nome, um número de id e um cargo/função</t>
-  </si>
-  <si>
     <t>R06</t>
   </si>
   <si>
@@ -151,6 +145,42 @@
   </si>
   <si>
     <t>R08.1</t>
+  </si>
+  <si>
+    <t>R10</t>
+  </si>
+  <si>
+    <t>25/09/202410:16</t>
+  </si>
+  <si>
+    <t>Deve ser possível gerir os funcionários da competição</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JF </t>
+  </si>
+  <si>
+    <t>R11</t>
+  </si>
+  <si>
+    <t>Deve ser possível adicionar, editar e remover atletas e treinadores antes do início da competição</t>
+  </si>
+  <si>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>Deve ser possível adicionar e editar os resultados das partidas</t>
+  </si>
+  <si>
+    <t>R13</t>
+  </si>
+  <si>
+    <t>R05.1</t>
+  </si>
+  <si>
+    <t>Cada funcionário tem um nome, um número de id e um cargo/função (juíz, camera, auxiliar)</t>
+  </si>
+  <si>
+    <t>Cada partida acontecerá a uma determinada hora, entre duas ou mais equipes</t>
   </si>
 </sst>
 </file>
@@ -430,7 +460,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -554,6 +584,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -771,15 +804,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.58203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.4140625" customWidth="1"/>
     <col min="2" max="2" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="64.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="79.9140625" customWidth="1"/>
     <col min="4" max="4" width="19.83203125" style="36" customWidth="1"/>
     <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.6640625" customWidth="1"/>
@@ -915,7 +948,7 @@
       <c r="B13" s="26">
         <v>45560.402083333334</v>
       </c>
-      <c r="C13" s="43" t="s">
+      <c r="C13" s="51" t="s">
         <v>30</v>
       </c>
       <c r="D13" s="22"/>
@@ -931,13 +964,13 @@
     </row>
     <row r="14" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="22" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="B14" s="26">
-        <v>45560.40347222222</v>
+        <v>45560.4375</v>
       </c>
       <c r="C14" s="40" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="D14" s="24"/>
       <c r="E14" s="22"/>
@@ -950,13 +983,13 @@
     </row>
     <row r="15" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="22" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B15" s="26">
         <v>45560.40902777778</v>
       </c>
       <c r="C15" s="39" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D15" s="22"/>
       <c r="E15" s="22" t="s">
@@ -971,13 +1004,13 @@
     </row>
     <row r="16" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16" s="22" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B16" s="32">
         <v>45560.409722222219</v>
       </c>
       <c r="C16" s="39" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D16" s="22"/>
       <c r="E16" s="22"/>
@@ -990,13 +1023,13 @@
     </row>
     <row r="17" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A17" s="22" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B17" s="32">
         <v>45560.416666666664</v>
       </c>
       <c r="C17" s="39" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D17" s="22"/>
       <c r="E17" s="22"/>
@@ -1009,13 +1042,13 @@
     </row>
     <row r="18" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A18" s="22" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B18" s="32">
         <v>45560.411805555559</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D18" s="22"/>
       <c r="E18" s="22"/>
@@ -1027,40 +1060,80 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="22"/>
-      <c r="B19" s="32"/>
-      <c r="C19" s="31"/>
+      <c r="A19" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="31" t="s">
+        <v>41</v>
+      </c>
       <c r="D19" s="22"/>
       <c r="E19" s="22"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="22"/>
+      <c r="F19" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="G19" s="22" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="20" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="22"/>
-      <c r="B20" s="26"/>
-      <c r="C20" s="39"/>
+      <c r="A20" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="26">
+        <v>45560.428472222222</v>
+      </c>
+      <c r="C20" s="39" t="s">
+        <v>44</v>
+      </c>
       <c r="D20" s="24"/>
       <c r="E20" s="22"/>
-      <c r="F20" s="24"/>
-      <c r="G20" s="22"/>
+      <c r="F20" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="G20" s="22" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="21" spans="1:7" ht="37.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="22"/>
-      <c r="B21" s="26"/>
-      <c r="C21" s="31"/>
+      <c r="A21" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="26">
+        <v>45560.430555555555</v>
+      </c>
+      <c r="C21" s="31" t="s">
+        <v>46</v>
+      </c>
       <c r="D21" s="27"/>
       <c r="E21" s="22"/>
-      <c r="F21" s="24"/>
-      <c r="G21" s="22"/>
+      <c r="F21" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="G21" s="22" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="22" spans="1:7" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="22"/>
-      <c r="B22" s="32"/>
-      <c r="C22" s="31"/>
+      <c r="A22" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" s="32">
+        <v>45560.438888888886</v>
+      </c>
+      <c r="C22" s="31" t="s">
+        <v>50</v>
+      </c>
       <c r="D22" s="24"/>
       <c r="E22" s="22"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="22"/>
+      <c r="F22" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="G22" s="22" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="23" spans="1:7" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="22"/>

</xml_diff>